<commit_message>
Added backend for funding graph
</commit_message>
<xml_diff>
--- a/frontend/public/template.xlsx
+++ b/frontend/public/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iitk-my.sharepoint.com/personal/rudradeep22_iitk_ac_in/Documents/Desktop/CarbonCalculator_Dashboard/frontend/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="11_F25DC773A252ABDACC104836D1DF79625ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DC2A190-55F8-4118-BC1F-A62CBBCFBE48}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_F25DC773A252ABDACC104836D1DF79625ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{907D9387-A5BB-4B0E-A870-0DAB8762F677}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Linkedin Posts</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Each row indicatesan OutReach event</t>
+  </si>
+  <si>
+    <t>Total Funding</t>
+  </si>
+  <si>
+    <t>Monthly Budget</t>
+  </si>
+  <si>
+    <t>Expenditure</t>
+  </si>
+  <si>
+    <t>Each cell represents budget for that month</t>
   </si>
 </sst>
 </file>
@@ -394,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,10 +419,13 @@
     <col min="3" max="3" width="33.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,8 +447,17 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -454,6 +478,9 @@
       </c>
       <c r="G2" t="s">
         <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>